<commit_message>
changed in test script
</commit_message>
<xml_diff>
--- a/WD_KeywordDrivenFramework/src/com/testscript/Test.xlsx
+++ b/WD_KeywordDrivenFramework/src/com/testscript/Test.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="39">
   <si>
     <t>RunMode</t>
   </si>
@@ -86,13 +86,52 @@
     <t>launchBrowser</t>
   </si>
   <si>
-    <t>VerifyPage</t>
-  </si>
-  <si>
-    <t>EnterText</t>
-  </si>
-  <si>
     <t>click</t>
+  </si>
+  <si>
+    <t>Test02</t>
+  </si>
+  <si>
+    <t>Test Gmail Login</t>
+  </si>
+  <si>
+    <t>End</t>
+  </si>
+  <si>
+    <t>TS_005</t>
+  </si>
+  <si>
+    <t>TS_006</t>
+  </si>
+  <si>
+    <t>TS_007</t>
+  </si>
+  <si>
+    <t>TS_008</t>
+  </si>
+  <si>
+    <t>Click on gmail link</t>
+  </si>
+  <si>
+    <t>verify the gmail login page should display</t>
+  </si>
+  <si>
+    <t>Enter text in username field</t>
+  </si>
+  <si>
+    <t>Enter text in password field</t>
+  </si>
+  <si>
+    <t>Click on Login Button</t>
+  </si>
+  <si>
+    <t>Verify that user should logged in</t>
+  </si>
+  <si>
+    <t>verifyPage</t>
+  </si>
+  <si>
+    <t>enterText</t>
   </si>
 </sst>
 </file>
@@ -181,6 +220,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -228,7 +270,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -263,7 +305,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -472,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,6 +553,17 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -519,10 +572,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,7 +641,7 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -602,7 +655,7 @@
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -616,7 +669,124 @@
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>